<commit_message>
Week 7 Experiment results
</commit_message>
<xml_diff>
--- a/project _list_android .xlsx
+++ b/project _list_android .xlsx
@@ -1235,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D58" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1253,7 +1253,7 @@
     <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>281</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1295,20 +1295,20 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
-        <f ca="1">RANDBETWEEN(550,2000)</f>
-        <v>1988</v>
-      </c>
-      <c r="G2">
-        <f ca="1">RANDBETWEEN(150,500)</f>
-        <v>352</v>
+      <c r="F2" s="1">
+        <v>1073</v>
+      </c>
+      <c r="G2" s="1">
+        <v>212</v>
       </c>
       <c r="H2" s="2">
-        <f ca="1">(G2/F2)*100</f>
-        <v>17.706237424547282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>19.757688723205966</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1325,19 +1325,19 @@
         <v>7</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F56" ca="1" si="0">RANDBETWEEN(550,2000)</f>
-        <v>1368</v>
+        <v>1963</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G56" ca="1" si="1">RANDBETWEEN(150,500)</f>
-        <v>362</v>
+        <v>171</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H56" ca="1" si="2">(G3/F3)*100</f>
-        <v>26.46198830409357</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>8.7111563932755978</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1354,19 +1354,19 @@
         <v>7</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>776</v>
+        <v>1942</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>430</v>
+        <v>478</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>55.412371134020624</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>24.613800205973224</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1383,19 +1383,19 @@
         <v>7</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>789</v>
+        <v>721</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>433</v>
+        <v>405</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>54.879594423320654</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>56.171983356449374</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1412,19 +1412,19 @@
         <v>7</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>673</v>
+        <v>724</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>214</v>
+        <v>307</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>31.797919762258541</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>42.403314917127069</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1441,19 +1441,19 @@
         <v>7</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>902</v>
+        <v>856</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>385</v>
+        <v>151</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42.68292682926829</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>17.640186915887853</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1470,19 +1470,19 @@
         <v>29</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1224</v>
+        <v>1689</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>240</v>
+        <v>481</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>19.607843137254903</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>28.478389579632918</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1499,19 +1499,19 @@
         <v>29</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1774</v>
+        <v>624</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>341</v>
+        <v>191</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>19.222096956031567</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>30.608974358974361</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1528,19 +1528,19 @@
         <v>37</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1218</v>
+        <v>1015</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>399</v>
+        <v>213</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>32.758620689655174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>20.985221674876847</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1557,19 +1557,19 @@
         <v>7</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1741</v>
+        <v>1964</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>469</v>
+        <v>167</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>26.938541068351523</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>8.5030549898167003</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1586,19 +1586,19 @@
         <v>7</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1263</v>
+        <v>1275</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>24.861441013460013</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>25.019607843137255</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1615,19 +1615,19 @@
         <v>7</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>786</v>
+        <v>724</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>187</v>
+        <v>305</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>23.791348600508904</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>42.127071823204417</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1644,19 +1644,19 @@
         <v>7</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1936</v>
+        <v>1563</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>17.613636363636363</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>22.200895713371722</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1673,19 +1673,19 @@
         <v>7</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1347</v>
+        <v>1954</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>319</v>
+        <v>179</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>23.682256867112102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>9.1606960081883315</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1702,19 +1702,19 @@
         <v>7</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1846</v>
+        <v>1869</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>491</v>
+        <v>425</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>26.59804983748646</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>22.739432851792401</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -1731,19 +1731,19 @@
         <v>7</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1809</v>
+        <v>568</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>380</v>
+        <v>345</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>21.006080707573243</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>60.739436619718312</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1760,19 +1760,19 @@
         <v>7</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1799</v>
+        <v>1932</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>290</v>
+        <v>193</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>16.120066703724291</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>9.9896480331262936</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1789,19 +1789,19 @@
         <v>7</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>812</v>
+        <v>1704</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>184</v>
+        <v>290</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>22.660098522167488</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>17.018779342723008</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1818,19 +1818,19 @@
         <v>7</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>938</v>
+        <v>1593</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>379</v>
+        <v>444</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40.405117270788914</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>27.871939736346519</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -1847,19 +1847,19 @@
         <v>78</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1209</v>
+        <v>1462</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>189</v>
+        <v>381</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>15.632754342431761</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>26.06019151846785</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1876,19 +1876,19 @@
         <v>83</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>962</v>
+        <v>1935</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>26.403326403326403</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>12.454780361757106</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -1905,19 +1905,19 @@
         <v>7</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1588</v>
+        <v>1684</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>357</v>
+        <v>464</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>22.481108312342567</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>27.553444180522561</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1934,19 +1934,19 @@
         <v>7</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>605</v>
+        <v>1280</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>342</v>
+        <v>235</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>56.528925619834716</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>18.359375</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -1963,19 +1963,19 @@
         <v>7</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1096</v>
+        <v>1337</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>172</v>
+        <v>244</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>15.693430656934307</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>18.249813014210918</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -1992,19 +1992,19 @@
         <v>7</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1476</v>
+        <v>1867</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>497</v>
+        <v>388</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>33.672086720867213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>20.782003213711835</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -2021,19 +2021,19 @@
         <v>7</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1389</v>
+        <v>1307</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>366</v>
+        <v>483</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>26.349892008639308</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>36.954858454475897</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -2050,19 +2050,19 @@
         <v>107</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1374</v>
+        <v>628</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>240</v>
+        <v>157</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>17.467248908296941</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>25</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2079,19 +2079,19 @@
         <v>111</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1388</v>
+        <v>1586</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>266</v>
+        <v>310</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>19.164265129682999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>19.546027742749054</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -2108,19 +2108,19 @@
         <v>7</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>726</v>
+        <v>1468</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>315</v>
+        <v>170</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>43.388429752066116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>11.580381471389646</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -2137,19 +2137,19 @@
         <v>7</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>705</v>
+        <v>1025</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>426</v>
+        <v>472</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.425531914893618</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>46.048780487804883</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -2166,19 +2166,19 @@
         <v>7</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1016</v>
+        <v>1434</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>394</v>
+        <v>255</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38.779527559055119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>17.782426778242677</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>124</v>
       </c>
@@ -2195,19 +2195,19 @@
         <v>7</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1593</v>
+        <v>1094</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>415</v>
+        <v>202</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>26.051475204017578</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>18.46435100548446</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>128</v>
       </c>
@@ -2224,19 +2224,19 @@
         <v>7</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>683</v>
+        <v>1594</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>283</v>
+        <v>230</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>41.434846266471446</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>14.429109159347552</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>130</v>
       </c>
@@ -2253,19 +2253,19 @@
         <v>7</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1005</v>
+        <v>1297</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>28.955223880597014</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>17.964533538936006</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>134</v>
       </c>
@@ -2282,19 +2282,19 @@
         <v>7</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1528</v>
+        <v>560</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>458</v>
+        <v>181</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>29.973821989528798</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>32.321428571428577</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>138</v>
       </c>
@@ -2311,19 +2311,19 @@
         <v>7</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>845</v>
+        <v>1207</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>488</v>
+        <v>359</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>57.751479289940832</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>29.743164871582433</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>142</v>
       </c>
@@ -2340,19 +2340,19 @@
         <v>145</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1031</v>
+        <v>1720</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>238</v>
+        <v>372</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>23.084384093113481</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>21.627906976744185</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -2369,19 +2369,19 @@
         <v>149</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>568</v>
+        <v>1578</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>341</v>
+        <v>275</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.035211267605639</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>17.427122940430927</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -2398,19 +2398,19 @@
         <v>7</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>563</v>
+        <v>1020</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>256</v>
+        <v>498</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>45.47069271758437</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>48.823529411764703</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -2427,19 +2427,19 @@
         <v>7</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1913</v>
+        <v>1271</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>382</v>
+        <v>474</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>19.968635650810246</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>37.293469708890633</v>
+      </c>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>158</v>
       </c>
@@ -2456,19 +2456,19 @@
         <v>162</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1006</v>
+        <v>1380</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>194</v>
+        <v>423</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>19.284294234592444</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>30.65217391304348</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>163</v>
       </c>
@@ -2485,19 +2485,19 @@
         <v>7</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1732</v>
+        <v>1895</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>212</v>
+        <v>494</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>12.240184757505773</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>26.068601583113455</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>167</v>
       </c>
@@ -2514,19 +2514,19 @@
         <v>7</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1132</v>
+        <v>1890</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>475</v>
+        <v>386</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>41.96113074204947</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>20.423280423280424</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>170</v>
       </c>
@@ -2543,19 +2543,19 @@
         <v>7</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1923</v>
+        <v>1605</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>367</v>
+        <v>304</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>19.084763390535624</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>18.940809968847354</v>
+      </c>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>174</v>
       </c>
@@ -2572,19 +2572,19 @@
         <v>7</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>797</v>
+        <v>1856</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>383</v>
+        <v>229</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>48.055207026348803</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>12.338362068965516</v>
+      </c>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>178</v>
       </c>
@@ -2601,19 +2601,19 @@
         <v>7</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>586</v>
+        <v>757</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>381</v>
+        <v>186</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>65.017064846416389</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>24.570673712021136</v>
+      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -2630,19 +2630,19 @@
         <v>7</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1286</v>
+        <v>1511</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>495</v>
+        <v>411</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38.491446345256605</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>27.200529450694905</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>186</v>
       </c>
@@ -2659,19 +2659,19 @@
         <v>7</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1957</v>
+        <v>1402</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>245</v>
+        <v>420</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>12.51916198262647</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>29.95720399429387</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>190</v>
       </c>
@@ -2688,19 +2688,19 @@
         <v>7</v>
       </c>
       <c r="F50" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1006</v>
+        <v>666</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>473</v>
+        <v>176</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>47.017892644135188</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>26.426426426426424</v>
+      </c>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>194</v>
       </c>
@@ -2717,19 +2717,19 @@
         <v>7</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>648</v>
+        <v>1517</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>211</v>
+        <v>408</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>32.561728395061728</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>26.895187870797628</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>197</v>
       </c>
@@ -2746,19 +2746,19 @@
         <v>7</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1285</v>
+        <v>1564</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>333</v>
+        <v>165</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>25.914396887159537</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>10.549872122762148</v>
+      </c>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>201</v>
       </c>
@@ -2775,19 +2775,19 @@
         <v>7</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>874</v>
+        <v>1476</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>161</v>
+        <v>280</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>18.421052631578945</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>18.97018970189702</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -2804,19 +2804,19 @@
         <v>7</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>660</v>
+        <v>1427</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>326</v>
+        <v>208</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>49.393939393939398</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>14.576033637000702</v>
+      </c>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>209</v>
       </c>
@@ -2833,19 +2833,19 @@
         <v>7</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>937</v>
+        <v>1159</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>278</v>
+        <v>498</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>29.669156883671295</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>42.968075927523728</v>
+      </c>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>213</v>
       </c>
@@ -2862,19 +2862,19 @@
         <v>7</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1213</v>
+        <v>949</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>215</v>
+        <v>164</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>17.724649629018963</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>17.281348788198102</v>
+      </c>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>216</v>
       </c>
@@ -2891,19 +2891,19 @@
         <v>7</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" ref="F57:F71" ca="1" si="3">RANDBETWEEN(550,2000)</f>
-        <v>1799</v>
+        <v>1445</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" ref="G57:G71" ca="1" si="4">RANDBETWEEN(150,500)</f>
-        <v>445</v>
+        <v>264</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" ref="H57:H73" ca="1" si="5">(G57/F57)*100</f>
-        <v>24.735964424680379</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+        <v>18.269896193771626</v>
+      </c>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>220</v>
       </c>
@@ -2920,19 +2920,19 @@
         <v>7</v>
       </c>
       <c r="F58" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1373</v>
+        <v>673</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>453</v>
+        <v>494</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>32.993445010924979</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+        <v>73.402674591381867</v>
+      </c>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>224</v>
       </c>
@@ -2949,19 +2949,19 @@
         <v>7</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1605</v>
+        <v>1301</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>355</v>
+        <v>481</v>
       </c>
       <c r="H59" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>22.118380062305295</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+        <v>36.971560338201378</v>
+      </c>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="2"/>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>228</v>
       </c>
@@ -2978,19 +2978,19 @@
         <v>7</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1430</v>
+        <v>1138</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>416</v>
+        <v>469</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>29.09090909090909</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>41.212653778558881</v>
+      </c>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="2"/>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>232</v>
       </c>
@@ -3007,19 +3007,19 @@
         <v>236</v>
       </c>
       <c r="F61" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1050</v>
+        <v>1519</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>235</v>
+        <v>401</v>
       </c>
       <c r="H61" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>22.380952380952383</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>26.398946675444375</v>
+      </c>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="2"/>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>237</v>
       </c>
@@ -3036,19 +3036,19 @@
         <v>7</v>
       </c>
       <c r="F62" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1211</v>
+        <v>1928</v>
       </c>
       <c r="G62" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>498</v>
+        <v>403</v>
       </c>
       <c r="H62" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>41.123038810900084</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>20.902489626556019</v>
+      </c>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="2"/>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>240</v>
       </c>
@@ -3065,19 +3065,19 @@
         <v>243</v>
       </c>
       <c r="F63" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1478</v>
+        <v>812</v>
       </c>
       <c r="G63" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>341</v>
+        <v>259</v>
       </c>
       <c r="H63" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>23.07171853856563</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>31.896551724137932</v>
+      </c>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="2"/>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>244</v>
       </c>
@@ -3094,19 +3094,19 @@
         <v>7</v>
       </c>
       <c r="F64" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1339</v>
+        <v>945</v>
       </c>
       <c r="G64" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>488</v>
+        <v>411</v>
       </c>
       <c r="H64" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>36.445108289768484</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+        <v>43.492063492063494</v>
+      </c>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="2"/>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" t="s">
         <v>248</v>
       </c>
@@ -3123,19 +3123,19 @@
         <v>7</v>
       </c>
       <c r="F65" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1680</v>
+        <v>699</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>383</v>
+        <v>320</v>
       </c>
       <c r="H65" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>22.797619047619047</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>45.779685264663804</v>
+      </c>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="2"/>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>252</v>
       </c>
@@ -3152,19 +3152,19 @@
         <v>7</v>
       </c>
       <c r="F66" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1139</v>
+        <v>1700</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>308</v>
+        <v>393</v>
       </c>
       <c r="H66" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>27.041264266900789</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>23.117647058823529</v>
+      </c>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="2"/>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>256</v>
       </c>
@@ -3181,19 +3181,19 @@
         <v>260</v>
       </c>
       <c r="F67" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1690</v>
+        <v>658</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>332</v>
+        <v>274</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>19.644970414201183</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>41.641337386018236</v>
+      </c>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="2"/>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>261</v>
       </c>
@@ -3210,19 +3210,19 @@
         <v>263</v>
       </c>
       <c r="F68" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>957</v>
+        <v>1103</v>
       </c>
       <c r="G68" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>260</v>
+        <v>423</v>
       </c>
       <c r="H68" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>27.168234064785789</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>38.349954669084312</v>
+      </c>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="2"/>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>264</v>
       </c>
@@ -3239,19 +3239,19 @@
         <v>7</v>
       </c>
       <c r="F69" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1292</v>
+        <v>1300</v>
       </c>
       <c r="G69" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>492</v>
+        <v>377</v>
       </c>
       <c r="H69" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>38.080495356037154</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>28.999999999999996</v>
+      </c>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="2"/>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>268</v>
       </c>
@@ -3268,19 +3268,19 @@
         <v>272</v>
       </c>
       <c r="F70" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>924</v>
+        <v>1848</v>
       </c>
       <c r="G70" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>201</v>
+        <v>271</v>
       </c>
       <c r="H70" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>21.753246753246753</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+        <v>14.664502164502164</v>
+      </c>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="2"/>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>273</v>
       </c>
@@ -3297,33 +3297,33 @@
         <v>276</v>
       </c>
       <c r="F71" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1881</v>
+        <v>1069</v>
       </c>
       <c r="G71" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="H71" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>12.387028176501861</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>20.95416276894294</v>
+      </c>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="2"/>
+    </row>
+    <row r="72" spans="1:11">
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
-      <c r="F73">
-        <f ca="1">SUM(F2:F72)</f>
-        <v>86142</v>
-      </c>
-      <c r="G73">
-        <f ca="1">SUM(G2:G72)</f>
-        <v>23669</v>
-      </c>
-      <c r="H73" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>27.47672447818718</v>
+    <row r="73" spans="1:11">
+      <c r="H73" s="2"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="F75">
+        <v>89596</v>
+      </c>
+      <c r="G75">
+        <v>21366</v>
+      </c>
+      <c r="H75">
+        <v>23.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>